<commit_message>
Added new test cases for Projects, Watchlists.
</commit_message>
<xml_diff>
--- a/src/test/test-data/WatchlistContainerTest.xlsx
+++ b/src/test/test-data/WatchlistContainerTest.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
   <sheets>
-    <sheet name="Watchlist" sheetId="1" r:id="rId1"/>
+    <sheet name="Watchlist Container" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="165">
   <si>
     <t>API</t>
   </si>
@@ -88,9 +88,6 @@
     <t>/people/search</t>
   </si>
   <si>
-    <t>OPQA-313</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -124,12 +121,6 @@
     <t>?itemType=wos</t>
   </si>
   <si>
-    <t>OPQA-1165</t>
-  </si>
-  <si>
-    <t>OPQA-1174</t>
-  </si>
-  <si>
     <t>Verify that to get patents for query</t>
   </si>
   <si>
@@ -163,9 +154,6 @@
     <t>Verify that user is able to create a new Watchlist using container API</t>
   </si>
   <si>
-    <t>OPQA-ZZZ</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that watchlist counts are shown as zero when user doesn't have any watchlists using container API. </t>
   </si>
   <si>
@@ -202,63 +190,27 @@
     <t>Verify that user is able to update watchlist description using container API</t>
   </si>
   <si>
-    <t>OPQA-AAA1</t>
-  </si>
-  <si>
-    <t>/container/(OPQA-AAA1_id)</t>
-  </si>
-  <si>
-    <t>OPQA-AAA2</t>
-  </si>
-  <si>
-    <t>OPQA-AAA3</t>
-  </si>
-  <si>
     <t>{ "desc": "Watchlist1 about cancer updated description from API" }</t>
   </si>
   <si>
     <t>status=200||type=watchlist||name=Watchlist1 about cancer updated from API||desc=Watchlist1 about cancer updated description from API||userid=(SYS_USER1)||ispublic=false</t>
   </si>
   <si>
-    <t>OPQA-AAA20</t>
-  </si>
-  <si>
     <t>Verify that user is able to delete existing watchlist using container API</t>
   </si>
   <si>
-    <t>OPQA-AAA21</t>
-  </si>
-  <si>
-    <t>/container/(OPQA-313_id)</t>
-  </si>
-  <si>
-    <t>OPQA-AAA4</t>
-  </si>
-  <si>
-    <t>OPQA-AAA5</t>
-  </si>
-  <si>
     <t>?itemType=all</t>
   </si>
   <si>
     <t>status=200||contents.patents=0||contents.wos=0||contents.posts=0||contents.documents=0||contents.dra_ss=0||contents.total=0</t>
   </si>
   <si>
-    <t>OPQA-AAA6</t>
-  </si>
-  <si>
     <t>Verify that user is able to make watchlist as public using container API</t>
   </si>
   <si>
     <t>{ "ispublic": true }</t>
   </si>
   <si>
-    <t>status=200||id=(OPQA-AAA1_id)||type=watchlist||userid=(SYS_USER1)||ispublic=true</t>
-  </si>
-  <si>
-    <t>OPQA-AAA7</t>
-  </si>
-  <si>
     <t>/container/contains/items</t>
   </si>
   <si>
@@ -268,96 +220,42 @@
     <t>{ "items" : [ {"id": "(OPQA-896_hits.hits[0]._id)", "type": "wos"}] }</t>
   </si>
   <si>
-    <t>OPQA-AAA1||OPQA-896</t>
-  </si>
-  <si>
     <t>?filter=count&amp;type=watchlist</t>
   </si>
   <si>
     <t>Verify that user is able to add an item to a particular watchlist using container API</t>
   </si>
   <si>
-    <t>/container/(OPQA-AAA1_id)/items</t>
-  </si>
-  <si>
-    <t>OPQA-AAA8</t>
-  </si>
-  <si>
     <t>Verify that user able to see any item watched status using container API</t>
   </si>
   <si>
-    <t>OPQA-AAA9</t>
-  </si>
-  <si>
     <t>Verify that user able to see added item watched status using container API</t>
   </si>
   <si>
-    <t>OPQA-AAA10</t>
-  </si>
-  <si>
-    <t>OPQA-AAA1||OPQA-896||OPQA-897||OPQA-898</t>
-  </si>
-  <si>
     <t>Verify that user is able to add multiple items like patent, post, wos to a particular watchlist using container API</t>
   </si>
   <si>
-    <t>OPQA-AAA11</t>
-  </si>
-  <si>
     <t>Verify that user is able to add multiple items like patent, post, wos to a multiple watchlists using container API</t>
   </si>
   <si>
-    <t>/container/(OPQA-313_id)/items</t>
-  </si>
-  <si>
-    <t>OPQA-313||OPQA-896||OPQA-897||OPQA-898</t>
-  </si>
-  <si>
     <t>Verify that user is able to remove an item from a particular watchlist using container API</t>
   </si>
   <si>
-    <t>/container/(OPQA-AAA1_id)/items/(OPQA-896_hits.hits[0]._id)</t>
-  </si>
-  <si>
-    <t>OPQA-AAA12</t>
-  </si>
-  <si>
-    <t>OPQA-AAA13</t>
-  </si>
-  <si>
     <t>Verify that container API returns list of user ids who are watching a particular item</t>
   </si>
   <si>
     <t>/container/items/contains/(OPQA-896_hits.hits[0]._id)</t>
   </si>
   <si>
-    <t>OPQA-AAA1||OPQA-313||OPQA-896</t>
-  </si>
-  <si>
-    <t>status=200||userId=(SYS_USER1)||containerId=(OPQA-AAA1_id)||containerId=(OPQA-313_id)</t>
-  </si>
-  <si>
-    <t>OPQA-AAA14</t>
-  </si>
-  <si>
     <t>Verify that user able to get item exists status properly for the removed item from particular watchlist using container API</t>
   </si>
   <si>
     <t>Verify that get container metadata and content works as expected using container API</t>
   </si>
   <si>
-    <t>status=200||id=(OPQA-AAA1_id)||type=watchlist||ispublic=true||contents.patents=2||contents.wos=2||contents.posts=2||contents.documents=0||contents.dra_ss=0||contents.total=6</t>
-  </si>
-  <si>
-    <t>Verify that deleted watchlist can't be deleted and check the error status using container API</t>
-  </si>
-  <si>
     <t>status=400</t>
   </si>
   <si>
-    <t>id=(OPQA-AAA1_id)||ispublic=false</t>
-  </si>
-  <si>
     <t>status=200||code=200</t>
   </si>
   <si>
@@ -370,13 +268,241 @@
     <t>status=200||(OPQA-896_hits.hits[0]._id).itemExists=true||(OPQA-896_hits.hits[0]._id).numberTotalContainers=2</t>
   </si>
   <si>
-    <t>OPQA-AAA13_1</t>
-  </si>
-  <si>
-    <t>/container/(OPQA-313_id)/items/(OPQA-896_hits.hits[0]._id)</t>
-  </si>
-  <si>
-    <t>OPQA-313||OPQA-896</t>
+    <t>Verify that deleted watchlist can't be deleted  and check the error status using container API</t>
+  </si>
+  <si>
+    <t>Verify that unauthorized member can't update watchlist's title or description and check the error status using container API</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER2)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>{ "name": "Watchlist1 about cancer updated from API", "desc": "Watchlist1 about cancer updated description from API" }</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400||Reason=Invalid containerId or User is not a container owner</t>
+  </si>
+  <si>
+    <t>Verify that unauthorized user is not able to add an item to others watchlist and check the error status using container API</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to remove an item from others watchlist and check the error status using container API</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to delete others watchlist and check the error status using container API</t>
+  </si>
+  <si>
+    <t>Verify that container metadata and content doesn't returned without passing userid and check the error status using container API</t>
+  </si>
+  <si>
+    <t>status=500||errorcode=500</t>
+  </si>
+  <si>
+    <t>Verify that Get the container data with sort option is works as expected using container API</t>
+  </si>
+  <si>
+    <t>status=200||type=wos||id=(OPQA-896_hits.hits[0]._id)||||id=(OPQA-896_hits.hits[1]._id)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that watchlist public, private counts are shown properly after updating the status using container API. </t>
+  </si>
+  <si>
+    <t>status=200||public_count=1||private_count=1||total_count=2</t>
+  </si>
+  <si>
+    <t>Verify that user is able to retrieve all item details for a particular watchlist using container API</t>
+  </si>
+  <si>
+    <t>status=200||content_items.id=(OPQA-896_hits.hits[0]._id)||content_items.id=(OPQA-896_hits.hits[1]._id)||content_items.id=(OPQA-897_hits.hits[0]._id)||content_items.id=(OPQA-897_hits.hits[1]._id)||content_items.id=(OPQA-898_hits.hits[0]._id)||content_items.id=(OPQA-898_hits.hits[1]._id)</t>
+  </si>
+  <si>
+    <t>Verify that user is able to retrieve only wos items details for a particular watchlist using container API</t>
+  </si>
+  <si>
+    <t>status=200||content_items.id=(OPQA-896_hits.hits[0]._id)||content_items.id=(OPQA-896_hits.hits[1]._id)||content_items[0].type=wos</t>
+  </si>
+  <si>
+    <t>Verify that get watchlist container details by group id works as expected using container API</t>
+  </si>
+  <si>
+    <t>Verify that get watchlist containers for a user works as expected using container API</t>
+  </si>
+  <si>
+    <t>public[0].groupid</t>
+  </si>
+  <si>
+    <t>Verify that user able to get item exists status properly for the removed item from particular watchlist using container's responseType as modal API</t>
+  </si>
+  <si>
+    <t>?responseType=modal&amp;type=watchlist</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400||Reason=Invalid containerId or User is not a container owner, or group member</t>
+  </si>
+  <si>
+    <t>OPQA-3992</t>
+  </si>
+  <si>
+    <t>OPQA-3993</t>
+  </si>
+  <si>
+    <t>/container/(OPQA-3993_id)</t>
+  </si>
+  <si>
+    <t>id=(OPQA-3993_id)||ispublic=false</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-3993_id)||type=watchlist||userid=(SYS_USER1)||ispublic=true</t>
+  </si>
+  <si>
+    <t>OPQA-3993||OPQA-896</t>
+  </si>
+  <si>
+    <t>/container/(OPQA-3993_id)/items</t>
+  </si>
+  <si>
+    <t>OPQA-3993||OPQA-896||OPQA-897||OPQA-898</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-3993_id)||type=watchlist||ispublic=true||contents.patents=2||contents.wos=2||contents.posts=2||contents.documents=0||contents.dra_ss=0||contents.total=6</t>
+  </si>
+  <si>
+    <t>/container/(OPQA-3993_id)/items?itemType=wos&amp;sortoption=latestupdated</t>
+  </si>
+  <si>
+    <t>/container/(OPQA-3993_id)/items/(OPQA-896_hits.hits[0]._id)</t>
+  </si>
+  <si>
+    <t>OPQA-3994</t>
+  </si>
+  <si>
+    <t>/container/(OPQA-3994_id)</t>
+  </si>
+  <si>
+    <t>/container/(OPQA-3994_id)/items</t>
+  </si>
+  <si>
+    <t>OPQA-3994||OPQA-896||OPQA-897||OPQA-898</t>
+  </si>
+  <si>
+    <t>OPQA-3993||OPQA-3994||OPQA-896</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER1)||containerId=(OPQA-3993_id)||containerId=(OPQA-3994_id)</t>
+  </si>
+  <si>
+    <t>OPQA-3993||OPQA-3994</t>
+  </si>
+  <si>
+    <t>status=200||public_count=1||private_count=1||total_count=2||public.id=(OPQA-3993_id)||private.id=(OPQA-3994_id)</t>
+  </si>
+  <si>
+    <t>/container/(OPQA-3994_id)/items/(OPQA-896_hits.hits[0]._id)</t>
+  </si>
+  <si>
+    <t>OPQA-3994||OPQA-896</t>
+  </si>
+  <si>
+    <t>OPQA-3995</t>
+  </si>
+  <si>
+    <t>OPQA-3996</t>
+  </si>
+  <si>
+    <t>OPQA-3997</t>
+  </si>
+  <si>
+    <t>OPQA-3998</t>
+  </si>
+  <si>
+    <t>OPQA-3999</t>
+  </si>
+  <si>
+    <t>OPQA-4000</t>
+  </si>
+  <si>
+    <t>OPQA-4000||OPQA-3994</t>
+  </si>
+  <si>
+    <t>OPQA-4001</t>
+  </si>
+  <si>
+    <t>OPQA-4002</t>
+  </si>
+  <si>
+    <t>OPQA-4003</t>
+  </si>
+  <si>
+    <t>OPQA-4004</t>
+  </si>
+  <si>
+    <t>OPQA-4005</t>
+  </si>
+  <si>
+    <t>OPQA-4006</t>
+  </si>
+  <si>
+    <t>OPQA-4007</t>
+  </si>
+  <si>
+    <t>OPQA-4008</t>
+  </si>
+  <si>
+    <t>OPQA-4009</t>
+  </si>
+  <si>
+    <t>/container/(SYS_USER1)/ByGroup/(OPQA-4009_public[0].groupid)</t>
+  </si>
+  <si>
+    <t>status=200||public.id=(OPQA-3993_id)||public.groupid=(OPQA-4009_public[0].groupid)||public.type=watchlist</t>
+  </si>
+  <si>
+    <t>OPQA-4010</t>
+  </si>
+  <si>
+    <t>OPQA-4011</t>
+  </si>
+  <si>
+    <t>OPQA-4012</t>
+  </si>
+  <si>
+    <t>OPQA-4013</t>
+  </si>
+  <si>
+    <t>OPQA-4014</t>
+  </si>
+  <si>
+    <t>OPQA-4015</t>
+  </si>
+  <si>
+    <t>OPQA-4016</t>
+  </si>
+  <si>
+    <t>OPQA-4016_1</t>
+  </si>
+  <si>
+    <t>OPQA-4017</t>
+  </si>
+  <si>
+    <t>OPQA-4018</t>
+  </si>
+  <si>
+    <t>OPQA-4019</t>
+  </si>
+  <si>
+    <t>OPQA-4020</t>
+  </si>
+  <si>
+    <t>OPQA-4021</t>
+  </si>
+  <si>
+    <t>OPQA-4020_1</t>
+  </si>
+  <si>
+    <t>OPQA-4022</t>
   </si>
   <si>
     <t/>
@@ -798,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L26"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -887,15 +1013,15 @@
         <v>21</v>
       </c>
       <c r="L2" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="30">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -908,7 +1034,7 @@
       </c>
       <c r="F3"/>
       <c r="G3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3"/>
@@ -919,15 +1045,15 @@
         <v>21</v>
       </c>
       <c r="L3" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="30">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
@@ -940,7 +1066,7 @@
       </c>
       <c r="F4"/>
       <c r="G4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4"/>
@@ -951,15 +1077,15 @@
         <v>21</v>
       </c>
       <c r="L4" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="15.75">
       <c r="A5" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
@@ -972,7 +1098,7 @@
       </c>
       <c r="F5"/>
       <c r="G5" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5"/>
@@ -983,721 +1109,1125 @@
         <v>13</v>
       </c>
       <c r="L5" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="47.25">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>109</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6"/>
       <c r="J6" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="300">
       <c r="A7" s="2" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="G7"/>
       <c r="H7" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I7"/>
       <c r="J7" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L7" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="120">
       <c r="A8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="G8"/>
       <c r="H8" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I8"/>
       <c r="J8" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L8" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="300">
       <c r="A9" s="2" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>63</v>
+        <v>111</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9"/>
       <c r="H9" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="105">
       <c r="A10" s="2" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>63</v>
+        <v>111</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10"/>
       <c r="H10" s="12" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="75">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="1" customFormat="1" ht="60">
       <c r="A11" s="2" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>1</v>
+        <v>111</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11"/>
+        <v>86</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="I11" s="2" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" ht="30">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1" ht="75">
       <c r="A12" s="2" t="s">
-        <v>73</v>
+        <v>133</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>63</v>
+        <v>111</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12"/>
+        <v>28</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="H12"/>
       <c r="I12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2"/>
+      <c r="L12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="1" customFormat="1" ht="30">
+      <c r="A13" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K13"/>
+      <c r="L13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="60">
+      <c r="A14" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14"/>
+      <c r="H14" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="K12"/>
-      <c r="L12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" ht="60">
-      <c r="A13" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13"/>
-      <c r="H13" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="75">
-      <c r="A14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H14" t="s">
-        <v>83</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" ht="60">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="1" customFormat="1" ht="47.25">
       <c r="A15" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>86</v>
+        <v>137</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>87</v>
+        <v>42</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" t="s">
-        <v>83</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>84</v>
+        <v>28</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="75">
       <c r="A16" s="2" t="s">
-        <v>90</v>
+        <v>138</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="G16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="H16" t="s">
-        <v>83</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="1" customFormat="1" ht="60">
       <c r="A17" s="2" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>115</v>
+        <v>47</v>
+      </c>
+      <c r="H17" t="s">
+        <v>67</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="1" customFormat="1" ht="60">
       <c r="A18" s="2" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="L18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="1" customFormat="1" ht="75">
+      <c r="A19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="13" t="s">
+      <c r="G19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="1" customFormat="1" ht="60">
+      <c r="A20" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="K18"/>
-      <c r="L18" t="s">
+      <c r="E20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="1" customFormat="1" ht="60">
+      <c r="A21" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" s="1" customFormat="1" ht="60">
-      <c r="A19" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="K19"/>
-      <c r="L19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="1" customFormat="1" ht="90">
-      <c r="A20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="K20"/>
-      <c r="L20" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="1" customFormat="1" ht="30">
-      <c r="A21" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21"/>
+        <v>47</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>81</v>
+      </c>
       <c r="I21" s="5" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="K21"/>
       <c r="L21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="1" customFormat="1" ht="30">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="1" customFormat="1" ht="60">
       <c r="A22" s="2" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22"/>
+      <c r="H22" s="13"/>
       <c r="I22" s="5" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="K22"/>
       <c r="L22" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="1" customFormat="1" ht="75">
       <c r="A23" s="2" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>25</v>
+        <v>43</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H23" t="s">
-        <v>83</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="H23" s="13"/>
       <c r="I23" s="2" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K23"/>
+        <v>127</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>105</v>
+      </c>
       <c r="L23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="30">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="1" customFormat="1" ht="90">
       <c r="A24" s="2" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>33</v>
+        <v>42</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G24"/>
-      <c r="H24" s="2"/>
+      <c r="H24"/>
       <c r="I24" s="2" t="s">
-        <v>62</v>
+        <v>143</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K24" s="2"/>
+        <v>117</v>
+      </c>
+      <c r="K24"/>
       <c r="L24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="30">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="1" customFormat="1" ht="45">
       <c r="A25" s="2" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>29</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="7"/>
       <c r="G25"/>
-      <c r="H25" s="2"/>
+      <c r="H25"/>
       <c r="I25" s="2" t="s">
-        <v>24</v>
+        <v>143</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="K25"/>
       <c r="L25" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="30">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="1" customFormat="1" ht="60">
       <c r="A26" s="2" t="s">
-        <v>37</v>
+        <v>150</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>71</v>
+        <v>42</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>29</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F26" s="7"/>
       <c r="G26"/>
-      <c r="H26" s="2"/>
+      <c r="H26"/>
       <c r="I26" s="2" t="s">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K26"/>
       <c r="L26" t="s">
-        <v>122</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="1" customFormat="1" ht="195">
+      <c r="A27" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27"/>
+      <c r="I27" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K27"/>
+      <c r="L27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="1" customFormat="1" ht="90">
+      <c r="A28" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28"/>
+      <c r="I28" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K28"/>
+      <c r="L28" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="1" customFormat="1" ht="60">
+      <c r="A29" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29"/>
+      <c r="I29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K29"/>
+      <c r="L29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="1" customFormat="1" ht="30">
+      <c r="A30" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30"/>
+      <c r="I30" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K30"/>
+      <c r="L30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="1" customFormat="1" ht="60">
+      <c r="A31" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31"/>
+      <c r="I31" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K31"/>
+      <c r="L31" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="1" customFormat="1" ht="30">
+      <c r="A32" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32"/>
+      <c r="I32" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K32"/>
+      <c r="L32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="1" customFormat="1" ht="75">
+      <c r="A33" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H33" t="s">
+        <v>67</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K33"/>
+      <c r="L33" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="1" customFormat="1" ht="75">
+      <c r="A34" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H34" t="s">
+        <v>67</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K34"/>
+      <c r="L34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="30">
+      <c r="A35" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K35" s="2"/>
+      <c r="L35" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="45">
+      <c r="A36" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G36"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K36" s="2"/>
+      <c r="L36" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="30">
+      <c r="A37" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K37"/>
+      <c r="L37" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="30">
+      <c r="A38" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K38"/>
+      <c r="L38" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>